<commit_message>
some sims were run with wrong power
</commit_message>
<xml_diff>
--- a/series_02/mpi_0/span_040/qsmf_output.xlsx
+++ b/series_02/mpi_0/span_040/qsmf_output.xlsx
@@ -395,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -536,10 +536,10 @@
         <v>-5</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>7.7875</v>
+        <v>7.7402</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -559,13 +559,13 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>6.7502</v>
+        <v>7.7143</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -585,27 +585,1015 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
+        <v>-3</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>7.3388</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>250</v>
+      </c>
+      <c r="F8">
+        <v>112</v>
+      </c>
+      <c r="G8">
+        <v>0.16</v>
+      </c>
+      <c r="H8">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>-2</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>6.5413</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>250</v>
+      </c>
+      <c r="F9">
+        <v>112</v>
+      </c>
+      <c r="G9">
+        <v>0.16</v>
+      </c>
+      <c r="H9">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>-1</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>5.0573</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>250</v>
+      </c>
+      <c r="F10">
+        <v>112</v>
+      </c>
+      <c r="G10">
+        <v>0.16</v>
+      </c>
+      <c r="H10">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>3.6659</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>250</v>
+      </c>
+      <c r="F11">
+        <v>112</v>
+      </c>
+      <c r="G11">
+        <v>0.16</v>
+      </c>
+      <c r="H11">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0.2982</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>250</v>
+      </c>
+      <c r="F12">
+        <v>112</v>
+      </c>
+      <c r="G12">
+        <v>0.16</v>
+      </c>
+      <c r="H12">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>-0.57316</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>250</v>
+      </c>
+      <c r="F13">
+        <v>112</v>
+      </c>
+      <c r="G13">
+        <v>0.16</v>
+      </c>
+      <c r="H13">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>-9</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>5.3205</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>250</v>
+      </c>
+      <c r="F14">
+        <v>112</v>
+      </c>
+      <c r="G14">
+        <v>0.16</v>
+      </c>
+      <c r="H14">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
         <v>-8</v>
       </c>
-      <c r="B8">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>6.1813</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>250</v>
+      </c>
+      <c r="F15">
+        <v>112</v>
+      </c>
+      <c r="G15">
+        <v>0.16</v>
+      </c>
+      <c r="H15">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>-7</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>6.8071</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>250</v>
+      </c>
+      <c r="F16">
+        <v>112</v>
+      </c>
+      <c r="G16">
+        <v>0.16</v>
+      </c>
+      <c r="H16">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>-6</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>7.3926</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>250</v>
+      </c>
+      <c r="F17">
+        <v>112</v>
+      </c>
+      <c r="G17">
+        <v>0.16</v>
+      </c>
+      <c r="H17">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>-5</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>7.7875</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>250</v>
+      </c>
+      <c r="F18">
+        <v>112</v>
+      </c>
+      <c r="G18">
+        <v>0.16</v>
+      </c>
+      <c r="H18">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>-4</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>7.9378</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>250</v>
+      </c>
+      <c r="F19">
+        <v>112</v>
+      </c>
+      <c r="G19">
+        <v>0.16</v>
+      </c>
+      <c r="H19">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>-3</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>7.5342</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>250</v>
+      </c>
+      <c r="F20">
+        <v>112</v>
+      </c>
+      <c r="G20">
+        <v>0.16</v>
+      </c>
+      <c r="H20">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>-2</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>6.9282</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>250</v>
+      </c>
+      <c r="F21">
+        <v>112</v>
+      </c>
+      <c r="G21">
+        <v>0.16</v>
+      </c>
+      <c r="H21">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>-1</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>6.104</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>250</v>
+      </c>
+      <c r="F22">
+        <v>112</v>
+      </c>
+      <c r="G22">
+        <v>0.16</v>
+      </c>
+      <c r="H22">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>3.2082</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>250</v>
+      </c>
+      <c r="F23">
+        <v>112</v>
+      </c>
+      <c r="G23">
+        <v>0.16</v>
+      </c>
+      <c r="H23">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>2.5765</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>250</v>
+      </c>
+      <c r="F24">
+        <v>112</v>
+      </c>
+      <c r="G24">
+        <v>0.16</v>
+      </c>
+      <c r="H24">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>-0.07762999999999999</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>250</v>
+      </c>
+      <c r="F25">
+        <v>112</v>
+      </c>
+      <c r="G25">
+        <v>0.16</v>
+      </c>
+      <c r="H25">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>-9</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>5.2825</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>250</v>
+      </c>
+      <c r="F26">
+        <v>112</v>
+      </c>
+      <c r="G26">
+        <v>0.16</v>
+      </c>
+      <c r="H26">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>-8</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>6.0249</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>250</v>
+      </c>
+      <c r="F27">
+        <v>112</v>
+      </c>
+      <c r="G27">
+        <v>0.16</v>
+      </c>
+      <c r="H27">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>-7</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>6.7502</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>250</v>
+      </c>
+      <c r="F28">
+        <v>112</v>
+      </c>
+      <c r="G28">
+        <v>0.16</v>
+      </c>
+      <c r="H28">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>-6</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>7.3621</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>250</v>
+      </c>
+      <c r="F29">
+        <v>112</v>
+      </c>
+      <c r="G29">
+        <v>0.16</v>
+      </c>
+      <c r="H29">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>-5</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>7.8595</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>250</v>
+      </c>
+      <c r="F30">
+        <v>112</v>
+      </c>
+      <c r="G30">
+        <v>0.16</v>
+      </c>
+      <c r="H30">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>-4</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>7.8952</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>250</v>
+      </c>
+      <c r="F31">
+        <v>112</v>
+      </c>
+      <c r="G31">
+        <v>0.16</v>
+      </c>
+      <c r="H31">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>-3</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>7.5713</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>250</v>
+      </c>
+      <c r="F32">
+        <v>112</v>
+      </c>
+      <c r="G32">
+        <v>0.16</v>
+      </c>
+      <c r="H32">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>-2</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>7.2009</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>250</v>
+      </c>
+      <c r="F33">
+        <v>112</v>
+      </c>
+      <c r="G33">
+        <v>0.16</v>
+      </c>
+      <c r="H33">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>-1</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>5.4998</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>250</v>
+      </c>
+      <c r="F34">
+        <v>112</v>
+      </c>
+      <c r="G34">
+        <v>0.16</v>
+      </c>
+      <c r="H34">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>4.7807</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>250</v>
+      </c>
+      <c r="F35">
+        <v>112</v>
+      </c>
+      <c r="G35">
+        <v>0.16</v>
+      </c>
+      <c r="H35">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>3.0644</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>250</v>
+      </c>
+      <c r="F36">
+        <v>112</v>
+      </c>
+      <c r="G36">
+        <v>0.16</v>
+      </c>
+      <c r="H36">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>2.2101</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>250</v>
+      </c>
+      <c r="F37">
+        <v>112</v>
+      </c>
+      <c r="G37">
+        <v>0.16</v>
+      </c>
+      <c r="H37">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38">
+        <v>-9</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>5.2036</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>250</v>
+      </c>
+      <c r="F38">
+        <v>112</v>
+      </c>
+      <c r="G38">
+        <v>0.16</v>
+      </c>
+      <c r="H38">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39">
+        <v>-8</v>
+      </c>
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>5.9503</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>250</v>
+      </c>
+      <c r="F39">
+        <v>112</v>
+      </c>
+      <c r="G39">
+        <v>0.16</v>
+      </c>
+      <c r="H39">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40">
+        <v>-7</v>
+      </c>
+      <c r="B40">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>6.629</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>250</v>
+      </c>
+      <c r="F40">
+        <v>112</v>
+      </c>
+      <c r="G40">
+        <v>0.16</v>
+      </c>
+      <c r="H40">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41">
+        <v>-6</v>
+      </c>
+      <c r="B41">
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <v>7.1449</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>250</v>
+      </c>
+      <c r="F41">
+        <v>112</v>
+      </c>
+      <c r="G41">
+        <v>0.16</v>
+      </c>
+      <c r="H41">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42">
+        <v>-5</v>
+      </c>
+      <c r="B42">
+        <v>12</v>
+      </c>
+      <c r="C42">
+        <v>7.6636</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>250</v>
+      </c>
+      <c r="F42">
+        <v>112</v>
+      </c>
+      <c r="G42">
+        <v>0.16</v>
+      </c>
+      <c r="H42">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43">
+        <v>-4</v>
+      </c>
+      <c r="B43">
+        <v>12</v>
+      </c>
+      <c r="C43">
+        <v>7.8713</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>250</v>
+      </c>
+      <c r="F43">
+        <v>112</v>
+      </c>
+      <c r="G43">
+        <v>0.16</v>
+      </c>
+      <c r="H43">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44">
+        <v>-3</v>
+      </c>
+      <c r="B44">
+        <v>12</v>
+      </c>
+      <c r="C44">
+        <v>7.9301</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>250</v>
+      </c>
+      <c r="F44">
+        <v>112</v>
+      </c>
+      <c r="G44">
+        <v>0.16</v>
+      </c>
+      <c r="H44">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45">
+        <v>-8</v>
+      </c>
+      <c r="B45">
         <v>24</v>
       </c>
-      <c r="C8">
+      <c r="C45">
         <v>5.5289</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>250</v>
-      </c>
-      <c r="F8">
-        <v>112</v>
-      </c>
-      <c r="G8">
-        <v>0.16</v>
-      </c>
-      <c r="H8">
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>250</v>
+      </c>
+      <c r="F45">
+        <v>112</v>
+      </c>
+      <c r="G45">
+        <v>0.16</v>
+      </c>
+      <c r="H45">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46">
+        <v>-9</v>
+      </c>
+      <c r="B46">
+        <v>40</v>
+      </c>
+      <c r="C46">
+        <v>4.6441</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>250</v>
+      </c>
+      <c r="F46">
+        <v>112</v>
+      </c>
+      <c r="G46">
+        <v>0.16</v>
+      </c>
+      <c r="H46">
         <v>0.158</v>
       </c>
     </row>

</xml_diff>

<commit_message>
span 40 data from hpc
</commit_message>
<xml_diff>
--- a/series_02/mpi_0/span_040/qsmf_output.xlsx
+++ b/series_02/mpi_0/span_040/qsmf_output.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,13 +435,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>6.9083</v>
+        <v>6.2348</v>
       </c>
       <c r="D2">
         <v>40</v>
@@ -464,13 +464,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>2</v>
+        <v>-7</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>-0.10562</v>
+        <v>6.9083</v>
       </c>
       <c r="D3">
         <v>40</v>
@@ -493,13 +493,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
-        <v>3</v>
+        <v>-6</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>-2.3532</v>
+        <v>7.4644</v>
       </c>
       <c r="D4">
         <v>40</v>
@@ -522,13 +522,13 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>6.1427</v>
+        <v>7.6675</v>
       </c>
       <c r="D5">
         <v>40</v>
@@ -551,13 +551,13 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6">
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>6.885</v>
+        <v>7.6557</v>
       </c>
       <c r="D6">
         <v>40</v>
@@ -580,13 +580,13 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7">
-        <v>-6</v>
+        <v>-3</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>7.4644</v>
+        <v>7.0835</v>
       </c>
       <c r="D7">
         <v>40</v>
@@ -609,13 +609,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>7.7595</v>
+        <v>6.3281</v>
       </c>
       <c r="D8">
         <v>40</v>
@@ -638,13 +638,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>7.9149</v>
+        <v>4.6601</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -667,13 +667,13 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>7.4954</v>
+        <v>4.7136</v>
       </c>
       <c r="D10">
         <v>40</v>
@@ -696,13 +696,13 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>6.3637</v>
+        <v>0.5385300000000001</v>
       </c>
       <c r="D11">
         <v>40</v>
@@ -725,13 +725,13 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>5.9177</v>
+        <v>-0.10562</v>
       </c>
       <c r="D12">
         <v>40</v>
@@ -754,13 +754,13 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>0.4539899999999999</v>
+        <v>-2.3532</v>
       </c>
       <c r="D13">
         <v>40</v>
@@ -783,13 +783,13 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14">
-        <v>3</v>
+        <v>-8</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14">
-        <v>-2.079</v>
+        <v>6.1427</v>
       </c>
       <c r="D14">
         <v>40</v>
@@ -812,13 +812,13 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15">
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>6.0446</v>
+        <v>6.885</v>
       </c>
       <c r="D15">
         <v>40</v>
@@ -841,13 +841,13 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16">
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="B16">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>6.7259</v>
+        <v>7.4644</v>
       </c>
       <c r="D16">
         <v>40</v>
@@ -870,13 +870,13 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>7.3102</v>
+        <v>7.7595</v>
       </c>
       <c r="D17">
         <v>40</v>
@@ -899,13 +899,13 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18">
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="B18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>7.8318</v>
+        <v>7.9149</v>
       </c>
       <c r="D18">
         <v>40</v>
@@ -928,13 +928,13 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="B19">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>7.9363</v>
+        <v>7.4954</v>
       </c>
       <c r="D19">
         <v>40</v>
@@ -960,10 +960,10 @@
         <v>-2</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>7.295</v>
+        <v>6.3637</v>
       </c>
       <c r="D20">
         <v>40</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="B21">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>7.8625</v>
+        <v>5.9177</v>
       </c>
       <c r="D21">
         <v>40</v>
@@ -1015,13 +1015,13 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>7.9658</v>
+        <v>3.9116</v>
       </c>
       <c r="D22">
         <v>40</v>
@@ -1044,13 +1044,13 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>7.4715</v>
+        <v>2.1783</v>
       </c>
       <c r="D23">
         <v>40</v>
@@ -1073,13 +1073,13 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C24">
-        <v>6.2922</v>
+        <v>0.4539899999999999</v>
       </c>
       <c r="D24">
         <v>40</v>
@@ -1102,13 +1102,13 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>5.4455</v>
+        <v>-2.079</v>
       </c>
       <c r="D25">
         <v>40</v>
@@ -1131,13 +1131,13 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26">
-        <v>1</v>
+        <v>-8</v>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C26">
-        <v>4.2317</v>
+        <v>6.0446</v>
       </c>
       <c r="D26">
         <v>40</v>
@@ -1160,13 +1160,13 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27">
-        <v>3</v>
+        <v>-7</v>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>-0.8363200000000001</v>
+        <v>6.7259</v>
       </c>
       <c r="D27">
         <v>40</v>
@@ -1192,10 +1192,10 @@
         <v>-6</v>
       </c>
       <c r="B28">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C28">
-        <v>7.1249</v>
+        <v>7.3102</v>
       </c>
       <c r="D28">
         <v>40</v>
@@ -1218,13 +1218,13 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29">
-        <v>2</v>
+        <v>-5</v>
       </c>
       <c r="B29">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C29">
-        <v>3.0525</v>
+        <v>7.8318</v>
       </c>
       <c r="D29">
         <v>40</v>
@@ -1247,13 +1247,13 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30">
-        <v>-8</v>
+        <v>-4</v>
       </c>
       <c r="B30">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C30">
-        <v>5.6211</v>
+        <v>7.9363</v>
       </c>
       <c r="D30">
         <v>40</v>
@@ -1276,13 +1276,13 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31">
-        <v>-7</v>
+        <v>-3</v>
       </c>
       <c r="B31">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C31">
-        <v>6.363</v>
+        <v>7.7374</v>
       </c>
       <c r="D31">
         <v>40</v>
@@ -1305,13 +1305,13 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32">
-        <v>-6</v>
+        <v>-2</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C32">
-        <v>6.8453</v>
+        <v>7.295</v>
       </c>
       <c r="D32">
         <v>40</v>
@@ -1334,13 +1334,13 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B33">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C33">
-        <v>7.8507</v>
+        <v>5.9288</v>
       </c>
       <c r="D33">
         <v>40</v>
@@ -1363,13 +1363,13 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C34">
-        <v>7.7819</v>
+        <v>2.7952</v>
       </c>
       <c r="D34">
         <v>40</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C35">
-        <v>7.2788</v>
+        <v>2.3159</v>
       </c>
       <c r="D35">
         <v>40</v>
@@ -1421,13 +1421,13 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B36">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C36">
-        <v>1.7103</v>
+        <v>0.9964499999999999</v>
       </c>
       <c r="D36">
         <v>40</v>
@@ -1450,13 +1450,13 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37">
-        <v>-8</v>
+        <v>3</v>
       </c>
       <c r="B37">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C37">
-        <v>5.5452</v>
+        <v>-0.1404</v>
       </c>
       <c r="D37">
         <v>40</v>
@@ -1479,13 +1479,13 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="B38">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C38">
-        <v>6.0478</v>
+        <v>5.8734</v>
       </c>
       <c r="D38">
         <v>40</v>
@@ -1508,13 +1508,13 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="B39">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C39">
-        <v>6.6921</v>
+        <v>6.5777</v>
       </c>
       <c r="D39">
         <v>40</v>
@@ -1537,13 +1537,13 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="B40">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C40">
-        <v>7.2427</v>
+        <v>7.112</v>
       </c>
       <c r="D40">
         <v>40</v>
@@ -1566,13 +1566,13 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="B41">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C41">
-        <v>7.5391</v>
+        <v>7.6874</v>
       </c>
       <c r="D41">
         <v>40</v>
@@ -1595,13 +1595,13 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="B42">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C42">
-        <v>7.8982</v>
+        <v>7.8625</v>
       </c>
       <c r="D42">
         <v>40</v>
@@ -1624,13 +1624,13 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="B43">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C43">
-        <v>7.842000000000001</v>
+        <v>7.9658</v>
       </c>
       <c r="D43">
         <v>40</v>
@@ -1653,13 +1653,13 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="B44">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C44">
-        <v>7.2961</v>
+        <v>7.4715</v>
       </c>
       <c r="D44">
         <v>40</v>
@@ -1682,13 +1682,13 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B45">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C45">
-        <v>6.3659</v>
+        <v>6.2922</v>
       </c>
       <c r="D45">
         <v>40</v>
@@ -1711,13 +1711,13 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B46">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C46">
-        <v>5.044</v>
+        <v>5.4455</v>
       </c>
       <c r="D46">
         <v>40</v>
@@ -1740,13 +1740,13 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B47">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C47">
-        <v>4.0013</v>
+        <v>4.2317</v>
       </c>
       <c r="D47">
         <v>40</v>
@@ -1769,13 +1769,13 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B48">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C48">
-        <v>2.8498</v>
+        <v>1.9038</v>
       </c>
       <c r="D48">
         <v>40</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49">
-        <v>-8</v>
+        <v>3</v>
       </c>
       <c r="B49">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C49">
-        <v>5.3858</v>
+        <v>-0.8363200000000001</v>
       </c>
       <c r="D49">
         <v>40</v>
@@ -1827,13 +1827,13 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="B50">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C50">
-        <v>6.0128</v>
+        <v>5.7662</v>
       </c>
       <c r="D50">
         <v>40</v>
@@ -1856,13 +1856,13 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="B51">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C51">
-        <v>6.4835</v>
+        <v>6.4491</v>
       </c>
       <c r="D51">
         <v>40</v>
@@ -1885,13 +1885,13 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="B52">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C52">
-        <v>7.0333</v>
+        <v>7.1249</v>
       </c>
       <c r="D52">
         <v>40</v>
@@ -1917,10 +1917,10 @@
         <v>-4</v>
       </c>
       <c r="B53">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C53">
-        <v>7.3343</v>
+        <v>7.7734</v>
       </c>
       <c r="D53">
         <v>40</v>
@@ -1946,10 +1946,10 @@
         <v>-3</v>
       </c>
       <c r="B54">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C54">
-        <v>7.7734</v>
+        <v>7.9363</v>
       </c>
       <c r="D54">
         <v>40</v>
@@ -1972,13 +1972,13 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="B55">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C55">
-        <v>7.6194</v>
+        <v>4.3096</v>
       </c>
       <c r="D55">
         <v>40</v>
@@ -2001,13 +2001,13 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="B56">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C56">
-        <v>7.468</v>
+        <v>3.0525</v>
       </c>
       <c r="D56">
         <v>40</v>
@@ -2030,13 +2030,13 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57">
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="B57">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C57">
-        <v>6.7985</v>
+        <v>5.6211</v>
       </c>
       <c r="D57">
         <v>40</v>
@@ -2059,30 +2059,1074 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58">
+        <v>-7</v>
+      </c>
+      <c r="B58">
+        <v>20</v>
+      </c>
+      <c r="C58">
+        <v>6.363</v>
+      </c>
+      <c r="D58">
+        <v>40</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>250</v>
+      </c>
+      <c r="G58">
+        <v>112</v>
+      </c>
+      <c r="H58">
+        <v>0.16</v>
+      </c>
+      <c r="I58">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59">
+        <v>-6</v>
+      </c>
+      <c r="B59">
+        <v>20</v>
+      </c>
+      <c r="C59">
+        <v>6.8453</v>
+      </c>
+      <c r="D59">
+        <v>40</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>250</v>
+      </c>
+      <c r="G59">
+        <v>112</v>
+      </c>
+      <c r="H59">
+        <v>0.16</v>
+      </c>
+      <c r="I59">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60">
+        <v>-3</v>
+      </c>
+      <c r="B60">
+        <v>20</v>
+      </c>
+      <c r="C60">
+        <v>7.8507</v>
+      </c>
+      <c r="D60">
+        <v>40</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>250</v>
+      </c>
+      <c r="G60">
+        <v>112</v>
+      </c>
+      <c r="H60">
+        <v>0.16</v>
+      </c>
+      <c r="I60">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61">
+        <v>-2</v>
+      </c>
+      <c r="B61">
+        <v>20</v>
+      </c>
+      <c r="C61">
+        <v>7.7819</v>
+      </c>
+      <c r="D61">
+        <v>40</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>250</v>
+      </c>
+      <c r="G61">
+        <v>112</v>
+      </c>
+      <c r="H61">
+        <v>0.16</v>
+      </c>
+      <c r="I61">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62">
+        <v>-1</v>
+      </c>
+      <c r="B62">
+        <v>20</v>
+      </c>
+      <c r="C62">
+        <v>7.2788</v>
+      </c>
+      <c r="D62">
+        <v>40</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>250</v>
+      </c>
+      <c r="G62">
+        <v>112</v>
+      </c>
+      <c r="H62">
+        <v>0.16</v>
+      </c>
+      <c r="I62">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63">
+        <v>3</v>
+      </c>
+      <c r="B63">
+        <v>20</v>
+      </c>
+      <c r="C63">
+        <v>1.7103</v>
+      </c>
+      <c r="D63">
+        <v>40</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>250</v>
+      </c>
+      <c r="G63">
+        <v>112</v>
+      </c>
+      <c r="H63">
+        <v>0.16</v>
+      </c>
+      <c r="I63">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64">
+        <v>-8</v>
+      </c>
+      <c r="B64">
+        <v>24</v>
+      </c>
+      <c r="C64">
+        <v>5.5452</v>
+      </c>
+      <c r="D64">
+        <v>40</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>250</v>
+      </c>
+      <c r="G64">
+        <v>112</v>
+      </c>
+      <c r="H64">
+        <v>0.16</v>
+      </c>
+      <c r="I64">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65">
+        <v>-7</v>
+      </c>
+      <c r="B65">
+        <v>24</v>
+      </c>
+      <c r="C65">
+        <v>6.0478</v>
+      </c>
+      <c r="D65">
+        <v>40</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>250</v>
+      </c>
+      <c r="G65">
+        <v>112</v>
+      </c>
+      <c r="H65">
+        <v>0.16</v>
+      </c>
+      <c r="I65">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66">
+        <v>-6</v>
+      </c>
+      <c r="B66">
+        <v>24</v>
+      </c>
+      <c r="C66">
+        <v>6.6921</v>
+      </c>
+      <c r="D66">
+        <v>40</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>250</v>
+      </c>
+      <c r="G66">
+        <v>112</v>
+      </c>
+      <c r="H66">
+        <v>0.16</v>
+      </c>
+      <c r="I66">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67">
+        <v>-5</v>
+      </c>
+      <c r="B67">
+        <v>24</v>
+      </c>
+      <c r="C67">
+        <v>7.2427</v>
+      </c>
+      <c r="D67">
+        <v>40</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>250</v>
+      </c>
+      <c r="G67">
+        <v>112</v>
+      </c>
+      <c r="H67">
+        <v>0.16</v>
+      </c>
+      <c r="I67">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68">
+        <v>-4</v>
+      </c>
+      <c r="B68">
+        <v>24</v>
+      </c>
+      <c r="C68">
+        <v>7.5391</v>
+      </c>
+      <c r="D68">
+        <v>40</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>250</v>
+      </c>
+      <c r="G68">
+        <v>112</v>
+      </c>
+      <c r="H68">
+        <v>0.16</v>
+      </c>
+      <c r="I68">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69">
+        <v>-3</v>
+      </c>
+      <c r="B69">
+        <v>24</v>
+      </c>
+      <c r="C69">
+        <v>7.8982</v>
+      </c>
+      <c r="D69">
+        <v>40</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>250</v>
+      </c>
+      <c r="G69">
+        <v>112</v>
+      </c>
+      <c r="H69">
+        <v>0.16</v>
+      </c>
+      <c r="I69">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70">
+        <v>-2</v>
+      </c>
+      <c r="B70">
+        <v>24</v>
+      </c>
+      <c r="C70">
+        <v>7.842000000000001</v>
+      </c>
+      <c r="D70">
+        <v>40</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>250</v>
+      </c>
+      <c r="G70">
+        <v>112</v>
+      </c>
+      <c r="H70">
+        <v>0.16</v>
+      </c>
+      <c r="I70">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71">
+        <v>-1</v>
+      </c>
+      <c r="B71">
+        <v>24</v>
+      </c>
+      <c r="C71">
+        <v>7.2961</v>
+      </c>
+      <c r="D71">
+        <v>40</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>250</v>
+      </c>
+      <c r="G71">
+        <v>112</v>
+      </c>
+      <c r="H71">
+        <v>0.16</v>
+      </c>
+      <c r="I71">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72">
+        <v>24</v>
+      </c>
+      <c r="C72">
+        <v>6.3659</v>
+      </c>
+      <c r="D72">
+        <v>40</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>250</v>
+      </c>
+      <c r="G72">
+        <v>112</v>
+      </c>
+      <c r="H72">
+        <v>0.16</v>
+      </c>
+      <c r="I72">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73">
         <v>1</v>
       </c>
-      <c r="B58">
+      <c r="B73">
+        <v>24</v>
+      </c>
+      <c r="C73">
+        <v>5.044</v>
+      </c>
+      <c r="D73">
+        <v>40</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>250</v>
+      </c>
+      <c r="G73">
+        <v>112</v>
+      </c>
+      <c r="H73">
+        <v>0.16</v>
+      </c>
+      <c r="I73">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74">
+        <v>2</v>
+      </c>
+      <c r="B74">
+        <v>24</v>
+      </c>
+      <c r="C74">
+        <v>4.0013</v>
+      </c>
+      <c r="D74">
+        <v>40</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>250</v>
+      </c>
+      <c r="G74">
+        <v>112</v>
+      </c>
+      <c r="H74">
+        <v>0.16</v>
+      </c>
+      <c r="I74">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>24</v>
+      </c>
+      <c r="C75">
+        <v>2.8498</v>
+      </c>
+      <c r="D75">
+        <v>40</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>250</v>
+      </c>
+      <c r="G75">
+        <v>112</v>
+      </c>
+      <c r="H75">
+        <v>0.16</v>
+      </c>
+      <c r="I75">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76">
+        <v>-8</v>
+      </c>
+      <c r="B76">
         <v>28</v>
       </c>
-      <c r="C58">
+      <c r="C76">
+        <v>5.3858</v>
+      </c>
+      <c r="D76">
+        <v>40</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>250</v>
+      </c>
+      <c r="G76">
+        <v>112</v>
+      </c>
+      <c r="H76">
+        <v>0.16</v>
+      </c>
+      <c r="I76">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77">
+        <v>-7</v>
+      </c>
+      <c r="B77">
+        <v>28</v>
+      </c>
+      <c r="C77">
+        <v>6.0128</v>
+      </c>
+      <c r="D77">
+        <v>40</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>250</v>
+      </c>
+      <c r="G77">
+        <v>112</v>
+      </c>
+      <c r="H77">
+        <v>0.16</v>
+      </c>
+      <c r="I77">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78">
+        <v>-6</v>
+      </c>
+      <c r="B78">
+        <v>28</v>
+      </c>
+      <c r="C78">
+        <v>6.4835</v>
+      </c>
+      <c r="D78">
+        <v>40</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>250</v>
+      </c>
+      <c r="G78">
+        <v>112</v>
+      </c>
+      <c r="H78">
+        <v>0.16</v>
+      </c>
+      <c r="I78">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79">
+        <v>-5</v>
+      </c>
+      <c r="B79">
+        <v>28</v>
+      </c>
+      <c r="C79">
+        <v>7.0333</v>
+      </c>
+      <c r="D79">
+        <v>40</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>250</v>
+      </c>
+      <c r="G79">
+        <v>112</v>
+      </c>
+      <c r="H79">
+        <v>0.16</v>
+      </c>
+      <c r="I79">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80">
+        <v>-4</v>
+      </c>
+      <c r="B80">
+        <v>28</v>
+      </c>
+      <c r="C80">
+        <v>7.3343</v>
+      </c>
+      <c r="D80">
+        <v>40</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>250</v>
+      </c>
+      <c r="G80">
+        <v>112</v>
+      </c>
+      <c r="H80">
+        <v>0.16</v>
+      </c>
+      <c r="I80">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81">
+        <v>-3</v>
+      </c>
+      <c r="B81">
+        <v>28</v>
+      </c>
+      <c r="C81">
+        <v>7.7734</v>
+      </c>
+      <c r="D81">
+        <v>40</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>250</v>
+      </c>
+      <c r="G81">
+        <v>112</v>
+      </c>
+      <c r="H81">
+        <v>0.16</v>
+      </c>
+      <c r="I81">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82">
+        <v>-2</v>
+      </c>
+      <c r="B82">
+        <v>28</v>
+      </c>
+      <c r="C82">
+        <v>7.6194</v>
+      </c>
+      <c r="D82">
+        <v>40</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>250</v>
+      </c>
+      <c r="G82">
+        <v>112</v>
+      </c>
+      <c r="H82">
+        <v>0.16</v>
+      </c>
+      <c r="I82">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83">
+        <v>-1</v>
+      </c>
+      <c r="B83">
+        <v>28</v>
+      </c>
+      <c r="C83">
+        <v>7.468</v>
+      </c>
+      <c r="D83">
+        <v>40</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>250</v>
+      </c>
+      <c r="G83">
+        <v>112</v>
+      </c>
+      <c r="H83">
+        <v>0.16</v>
+      </c>
+      <c r="I83">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84">
+        <v>0</v>
+      </c>
+      <c r="B84">
+        <v>28</v>
+      </c>
+      <c r="C84">
+        <v>6.7985</v>
+      </c>
+      <c r="D84">
+        <v>40</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>250</v>
+      </c>
+      <c r="G84">
+        <v>112</v>
+      </c>
+      <c r="H84">
+        <v>0.16</v>
+      </c>
+      <c r="I84">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85">
+        <v>1</v>
+      </c>
+      <c r="B85">
+        <v>28</v>
+      </c>
+      <c r="C85">
         <v>5.4609</v>
       </c>
-      <c r="D58">
-        <v>40</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58">
-        <v>250</v>
-      </c>
-      <c r="G58">
-        <v>112</v>
-      </c>
-      <c r="H58">
-        <v>0.16</v>
-      </c>
-      <c r="I58">
+      <c r="D85">
+        <v>40</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>250</v>
+      </c>
+      <c r="G85">
+        <v>112</v>
+      </c>
+      <c r="H85">
+        <v>0.16</v>
+      </c>
+      <c r="I85">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86">
+        <v>-8</v>
+      </c>
+      <c r="B86">
+        <v>32</v>
+      </c>
+      <c r="C86">
+        <v>5.2729</v>
+      </c>
+      <c r="D86">
+        <v>40</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>250</v>
+      </c>
+      <c r="G86">
+        <v>112</v>
+      </c>
+      <c r="H86">
+        <v>0.16</v>
+      </c>
+      <c r="I86">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87">
+        <v>-7</v>
+      </c>
+      <c r="B87">
+        <v>32</v>
+      </c>
+      <c r="C87">
+        <v>5.8297</v>
+      </c>
+      <c r="D87">
+        <v>40</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>250</v>
+      </c>
+      <c r="G87">
+        <v>112</v>
+      </c>
+      <c r="H87">
+        <v>0.16</v>
+      </c>
+      <c r="I87">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88">
+        <v>-6</v>
+      </c>
+      <c r="B88">
+        <v>32</v>
+      </c>
+      <c r="C88">
+        <v>6.2936</v>
+      </c>
+      <c r="D88">
+        <v>40</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>250</v>
+      </c>
+      <c r="G88">
+        <v>112</v>
+      </c>
+      <c r="H88">
+        <v>0.16</v>
+      </c>
+      <c r="I88">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89">
+        <v>-5</v>
+      </c>
+      <c r="B89">
+        <v>32</v>
+      </c>
+      <c r="C89">
+        <v>6.8114</v>
+      </c>
+      <c r="D89">
+        <v>40</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>250</v>
+      </c>
+      <c r="G89">
+        <v>112</v>
+      </c>
+      <c r="H89">
+        <v>0.16</v>
+      </c>
+      <c r="I89">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90">
+        <v>-4</v>
+      </c>
+      <c r="B90">
+        <v>32</v>
+      </c>
+      <c r="C90">
+        <v>7.2248</v>
+      </c>
+      <c r="D90">
+        <v>40</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>250</v>
+      </c>
+      <c r="G90">
+        <v>112</v>
+      </c>
+      <c r="H90">
+        <v>0.16</v>
+      </c>
+      <c r="I90">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91">
+        <v>-3</v>
+      </c>
+      <c r="B91">
+        <v>32</v>
+      </c>
+      <c r="C91">
+        <v>7.5452</v>
+      </c>
+      <c r="D91">
+        <v>40</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>250</v>
+      </c>
+      <c r="G91">
+        <v>112</v>
+      </c>
+      <c r="H91">
+        <v>0.16</v>
+      </c>
+      <c r="I91">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92">
+        <v>1</v>
+      </c>
+      <c r="B92">
+        <v>32</v>
+      </c>
+      <c r="C92">
+        <v>5.9559</v>
+      </c>
+      <c r="D92">
+        <v>40</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>250</v>
+      </c>
+      <c r="G92">
+        <v>112</v>
+      </c>
+      <c r="H92">
+        <v>0.16</v>
+      </c>
+      <c r="I92">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93">
+        <v>-4</v>
+      </c>
+      <c r="B93">
+        <v>36</v>
+      </c>
+      <c r="C93">
+        <v>6.952000000000001</v>
+      </c>
+      <c r="D93">
+        <v>40</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>250</v>
+      </c>
+      <c r="G93">
+        <v>112</v>
+      </c>
+      <c r="H93">
+        <v>0.16</v>
+      </c>
+      <c r="I93">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94">
+        <v>-2</v>
+      </c>
+      <c r="B94">
+        <v>36</v>
+      </c>
+      <c r="C94">
+        <v>7.661</v>
+      </c>
+      <c r="D94">
+        <v>40</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>250</v>
+      </c>
+      <c r="G94">
+        <v>112</v>
+      </c>
+      <c r="H94">
+        <v>0.16</v>
+      </c>
+      <c r="I94">
         <v>0.158</v>
       </c>
     </row>

</xml_diff>

<commit_message>
span 40 done in 4 jobs
</commit_message>
<xml_diff>
--- a/series_02/mpi_0/span_040/qsmf_output.xlsx
+++ b/series_02/mpi_0/span_040/qsmf_output.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1914,13 +1914,13 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="B53">
         <v>16</v>
       </c>
       <c r="C53">
-        <v>7.7734</v>
+        <v>7.4846</v>
       </c>
       <c r="D53">
         <v>40</v>
@@ -1943,13 +1943,13 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="B54">
         <v>16</v>
       </c>
       <c r="C54">
-        <v>7.9363</v>
+        <v>7.7734</v>
       </c>
       <c r="D54">
         <v>40</v>
@@ -1972,13 +1972,13 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="B55">
         <v>16</v>
       </c>
       <c r="C55">
-        <v>4.3096</v>
+        <v>7.9363</v>
       </c>
       <c r="D55">
         <v>40</v>
@@ -2001,13 +2001,13 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B56">
         <v>16</v>
       </c>
       <c r="C56">
-        <v>3.0525</v>
+        <v>7.6349</v>
       </c>
       <c r="D56">
         <v>40</v>
@@ -2030,13 +2030,13 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57">
-        <v>-8</v>
+        <v>-1</v>
       </c>
       <c r="B57">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C57">
-        <v>5.6211</v>
+        <v>7.0059</v>
       </c>
       <c r="D57">
         <v>40</v>
@@ -2059,13 +2059,13 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58">
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C58">
-        <v>6.363</v>
+        <v>6.2971</v>
       </c>
       <c r="D58">
         <v>40</v>
@@ -2088,13 +2088,13 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59">
-        <v>-6</v>
+        <v>1</v>
       </c>
       <c r="B59">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C59">
-        <v>6.8453</v>
+        <v>4.3096</v>
       </c>
       <c r="D59">
         <v>40</v>
@@ -2117,13 +2117,13 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="B60">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C60">
-        <v>7.8507</v>
+        <v>3.0525</v>
       </c>
       <c r="D60">
         <v>40</v>
@@ -2146,13 +2146,13 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="B61">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C61">
-        <v>7.7819</v>
+        <v>1.4243</v>
       </c>
       <c r="D61">
         <v>40</v>
@@ -2175,13 +2175,13 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62">
-        <v>-1</v>
+        <v>-8</v>
       </c>
       <c r="B62">
         <v>20</v>
       </c>
       <c r="C62">
-        <v>7.2788</v>
+        <v>5.6211</v>
       </c>
       <c r="D62">
         <v>40</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63">
-        <v>3</v>
+        <v>-7</v>
       </c>
       <c r="B63">
         <v>20</v>
       </c>
       <c r="C63">
-        <v>1.7103</v>
+        <v>6.363</v>
       </c>
       <c r="D63">
         <v>40</v>
@@ -2233,13 +2233,13 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64">
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="B64">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C64">
-        <v>5.5452</v>
+        <v>6.8453</v>
       </c>
       <c r="D64">
         <v>40</v>
@@ -2262,13 +2262,13 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65">
-        <v>-7</v>
+        <v>-5</v>
       </c>
       <c r="B65">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C65">
-        <v>6.0478</v>
+        <v>7.3189</v>
       </c>
       <c r="D65">
         <v>40</v>
@@ -2291,13 +2291,13 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="B66">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C66">
-        <v>6.6921</v>
+        <v>7.7903</v>
       </c>
       <c r="D66">
         <v>40</v>
@@ -2320,13 +2320,13 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="B67">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C67">
-        <v>7.2427</v>
+        <v>7.8507</v>
       </c>
       <c r="D67">
         <v>40</v>
@@ -2349,13 +2349,13 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="B68">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C68">
-        <v>7.5391</v>
+        <v>7.7819</v>
       </c>
       <c r="D68">
         <v>40</v>
@@ -2378,13 +2378,13 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B69">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C69">
-        <v>7.8982</v>
+        <v>7.2788</v>
       </c>
       <c r="D69">
         <v>40</v>
@@ -2407,13 +2407,13 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="B70">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C70">
-        <v>7.842000000000001</v>
+        <v>6.6426</v>
       </c>
       <c r="D70">
         <v>40</v>
@@ -2436,13 +2436,13 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B71">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C71">
-        <v>7.2961</v>
+        <v>4.9959</v>
       </c>
       <c r="D71">
         <v>40</v>
@@ -2465,13 +2465,13 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B72">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C72">
-        <v>6.3659</v>
+        <v>3.0273</v>
       </c>
       <c r="D72">
         <v>40</v>
@@ -2494,13 +2494,13 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B73">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C73">
-        <v>5.044</v>
+        <v>1.7103</v>
       </c>
       <c r="D73">
         <v>40</v>
@@ -2523,13 +2523,13 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74">
-        <v>2</v>
+        <v>-8</v>
       </c>
       <c r="B74">
         <v>24</v>
       </c>
       <c r="C74">
-        <v>4.0013</v>
+        <v>5.5452</v>
       </c>
       <c r="D74">
         <v>40</v>
@@ -2552,13 +2552,13 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75">
-        <v>3</v>
+        <v>-7</v>
       </c>
       <c r="B75">
         <v>24</v>
       </c>
       <c r="C75">
-        <v>2.8498</v>
+        <v>6.0478</v>
       </c>
       <c r="D75">
         <v>40</v>
@@ -2581,13 +2581,13 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76">
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="B76">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C76">
-        <v>5.3858</v>
+        <v>6.6921</v>
       </c>
       <c r="D76">
         <v>40</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77">
-        <v>-7</v>
+        <v>-5</v>
       </c>
       <c r="B77">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C77">
-        <v>6.0128</v>
+        <v>7.2427</v>
       </c>
       <c r="D77">
         <v>40</v>
@@ -2639,13 +2639,13 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="B78">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C78">
-        <v>6.4835</v>
+        <v>7.5391</v>
       </c>
       <c r="D78">
         <v>40</v>
@@ -2668,13 +2668,13 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="B79">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C79">
-        <v>7.0333</v>
+        <v>7.8982</v>
       </c>
       <c r="D79">
         <v>40</v>
@@ -2697,13 +2697,13 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="B80">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C80">
-        <v>7.3343</v>
+        <v>7.842000000000001</v>
       </c>
       <c r="D80">
         <v>40</v>
@@ -2726,13 +2726,13 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B81">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C81">
-        <v>7.7734</v>
+        <v>7.2961</v>
       </c>
       <c r="D81">
         <v>40</v>
@@ -2755,13 +2755,13 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="B82">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C82">
-        <v>7.6194</v>
+        <v>6.3659</v>
       </c>
       <c r="D82">
         <v>40</v>
@@ -2784,13 +2784,13 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B83">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C83">
-        <v>7.468</v>
+        <v>5.044</v>
       </c>
       <c r="D83">
         <v>40</v>
@@ -2813,13 +2813,13 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B84">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C84">
-        <v>6.7985</v>
+        <v>4.0013</v>
       </c>
       <c r="D84">
         <v>40</v>
@@ -2842,13 +2842,13 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B85">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C85">
-        <v>5.4609</v>
+        <v>2.8498</v>
       </c>
       <c r="D85">
         <v>40</v>
@@ -2874,10 +2874,10 @@
         <v>-8</v>
       </c>
       <c r="B86">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C86">
-        <v>5.2729</v>
+        <v>5.3858</v>
       </c>
       <c r="D86">
         <v>40</v>
@@ -2903,10 +2903,10 @@
         <v>-7</v>
       </c>
       <c r="B87">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C87">
-        <v>5.8297</v>
+        <v>6.0128</v>
       </c>
       <c r="D87">
         <v>40</v>
@@ -2932,10 +2932,10 @@
         <v>-6</v>
       </c>
       <c r="B88">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C88">
-        <v>6.2936</v>
+        <v>6.4835</v>
       </c>
       <c r="D88">
         <v>40</v>
@@ -2961,10 +2961,10 @@
         <v>-5</v>
       </c>
       <c r="B89">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C89">
-        <v>6.8114</v>
+        <v>7.0333</v>
       </c>
       <c r="D89">
         <v>40</v>
@@ -2990,10 +2990,10 @@
         <v>-4</v>
       </c>
       <c r="B90">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C90">
-        <v>7.2248</v>
+        <v>7.3343</v>
       </c>
       <c r="D90">
         <v>40</v>
@@ -3019,10 +3019,10 @@
         <v>-3</v>
       </c>
       <c r="B91">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C91">
-        <v>7.5452</v>
+        <v>7.7734</v>
       </c>
       <c r="D91">
         <v>40</v>
@@ -3045,13 +3045,13 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="B92">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C92">
-        <v>5.9559</v>
+        <v>7.6194</v>
       </c>
       <c r="D92">
         <v>40</v>
@@ -3074,13 +3074,13 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="B93">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C93">
-        <v>6.952000000000001</v>
+        <v>7.468</v>
       </c>
       <c r="D93">
         <v>40</v>
@@ -3103,30 +3103,1161 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94">
+        <v>0</v>
+      </c>
+      <c r="B94">
+        <v>28</v>
+      </c>
+      <c r="C94">
+        <v>6.7985</v>
+      </c>
+      <c r="D94">
+        <v>40</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>250</v>
+      </c>
+      <c r="G94">
+        <v>112</v>
+      </c>
+      <c r="H94">
+        <v>0.16</v>
+      </c>
+      <c r="I94">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95">
+        <v>1</v>
+      </c>
+      <c r="B95">
+        <v>28</v>
+      </c>
+      <c r="C95">
+        <v>5.4609</v>
+      </c>
+      <c r="D95">
+        <v>40</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>250</v>
+      </c>
+      <c r="G95">
+        <v>112</v>
+      </c>
+      <c r="H95">
+        <v>0.16</v>
+      </c>
+      <c r="I95">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96">
+        <v>2</v>
+      </c>
+      <c r="B96">
+        <v>28</v>
+      </c>
+      <c r="C96">
+        <v>4.6299</v>
+      </c>
+      <c r="D96">
+        <v>40</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>250</v>
+      </c>
+      <c r="G96">
+        <v>112</v>
+      </c>
+      <c r="H96">
+        <v>0.16</v>
+      </c>
+      <c r="I96">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97">
+        <v>3</v>
+      </c>
+      <c r="B97">
+        <v>28</v>
+      </c>
+      <c r="C97">
+        <v>3.7692</v>
+      </c>
+      <c r="D97">
+        <v>40</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>250</v>
+      </c>
+      <c r="G97">
+        <v>112</v>
+      </c>
+      <c r="H97">
+        <v>0.16</v>
+      </c>
+      <c r="I97">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98">
+        <v>-8</v>
+      </c>
+      <c r="B98">
+        <v>32</v>
+      </c>
+      <c r="C98">
+        <v>5.2729</v>
+      </c>
+      <c r="D98">
+        <v>40</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>250</v>
+      </c>
+      <c r="G98">
+        <v>112</v>
+      </c>
+      <c r="H98">
+        <v>0.16</v>
+      </c>
+      <c r="I98">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99">
+        <v>-7</v>
+      </c>
+      <c r="B99">
+        <v>32</v>
+      </c>
+      <c r="C99">
+        <v>5.8297</v>
+      </c>
+      <c r="D99">
+        <v>40</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>250</v>
+      </c>
+      <c r="G99">
+        <v>112</v>
+      </c>
+      <c r="H99">
+        <v>0.16</v>
+      </c>
+      <c r="I99">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100">
+        <v>-6</v>
+      </c>
+      <c r="B100">
+        <v>32</v>
+      </c>
+      <c r="C100">
+        <v>6.2936</v>
+      </c>
+      <c r="D100">
+        <v>40</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>250</v>
+      </c>
+      <c r="G100">
+        <v>112</v>
+      </c>
+      <c r="H100">
+        <v>0.16</v>
+      </c>
+      <c r="I100">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101">
+        <v>-5</v>
+      </c>
+      <c r="B101">
+        <v>32</v>
+      </c>
+      <c r="C101">
+        <v>6.8114</v>
+      </c>
+      <c r="D101">
+        <v>40</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>250</v>
+      </c>
+      <c r="G101">
+        <v>112</v>
+      </c>
+      <c r="H101">
+        <v>0.16</v>
+      </c>
+      <c r="I101">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102">
+        <v>-4</v>
+      </c>
+      <c r="B102">
+        <v>32</v>
+      </c>
+      <c r="C102">
+        <v>7.2248</v>
+      </c>
+      <c r="D102">
+        <v>40</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>250</v>
+      </c>
+      <c r="G102">
+        <v>112</v>
+      </c>
+      <c r="H102">
+        <v>0.16</v>
+      </c>
+      <c r="I102">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103">
+        <v>-3</v>
+      </c>
+      <c r="B103">
+        <v>32</v>
+      </c>
+      <c r="C103">
+        <v>7.5452</v>
+      </c>
+      <c r="D103">
+        <v>40</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>250</v>
+      </c>
+      <c r="G103">
+        <v>112</v>
+      </c>
+      <c r="H103">
+        <v>0.16</v>
+      </c>
+      <c r="I103">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104">
         <v>-2</v>
       </c>
-      <c r="B94">
+      <c r="B104">
+        <v>32</v>
+      </c>
+      <c r="C104">
+        <v>7.5965</v>
+      </c>
+      <c r="D104">
+        <v>40</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>250</v>
+      </c>
+      <c r="G104">
+        <v>112</v>
+      </c>
+      <c r="H104">
+        <v>0.16</v>
+      </c>
+      <c r="I104">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105">
+        <v>-1</v>
+      </c>
+      <c r="B105">
+        <v>32</v>
+      </c>
+      <c r="C105">
+        <v>7.487</v>
+      </c>
+      <c r="D105">
+        <v>40</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>250</v>
+      </c>
+      <c r="G105">
+        <v>112</v>
+      </c>
+      <c r="H105">
+        <v>0.16</v>
+      </c>
+      <c r="I105">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106">
+        <v>0</v>
+      </c>
+      <c r="B106">
+        <v>32</v>
+      </c>
+      <c r="C106">
+        <v>7.1671</v>
+      </c>
+      <c r="D106">
+        <v>40</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>250</v>
+      </c>
+      <c r="G106">
+        <v>112</v>
+      </c>
+      <c r="H106">
+        <v>0.16</v>
+      </c>
+      <c r="I106">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107">
+        <v>1</v>
+      </c>
+      <c r="B107">
+        <v>32</v>
+      </c>
+      <c r="C107">
+        <v>5.9559</v>
+      </c>
+      <c r="D107">
+        <v>40</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <v>250</v>
+      </c>
+      <c r="G107">
+        <v>112</v>
+      </c>
+      <c r="H107">
+        <v>0.16</v>
+      </c>
+      <c r="I107">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108">
+        <v>2</v>
+      </c>
+      <c r="B108">
+        <v>32</v>
+      </c>
+      <c r="C108">
+        <v>4.4702</v>
+      </c>
+      <c r="D108">
+        <v>40</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>250</v>
+      </c>
+      <c r="G108">
+        <v>112</v>
+      </c>
+      <c r="H108">
+        <v>0.16</v>
+      </c>
+      <c r="I108">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109">
+        <v>3</v>
+      </c>
+      <c r="B109">
+        <v>32</v>
+      </c>
+      <c r="C109">
+        <v>3.6645</v>
+      </c>
+      <c r="D109">
+        <v>40</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109">
+        <v>250</v>
+      </c>
+      <c r="G109">
+        <v>112</v>
+      </c>
+      <c r="H109">
+        <v>0.16</v>
+      </c>
+      <c r="I109">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110">
+        <v>-8</v>
+      </c>
+      <c r="B110">
         <v>36</v>
       </c>
-      <c r="C94">
+      <c r="C110">
+        <v>5.1883</v>
+      </c>
+      <c r="D110">
+        <v>40</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <v>250</v>
+      </c>
+      <c r="G110">
+        <v>112</v>
+      </c>
+      <c r="H110">
+        <v>0.16</v>
+      </c>
+      <c r="I110">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111">
+        <v>-7</v>
+      </c>
+      <c r="B111">
+        <v>36</v>
+      </c>
+      <c r="C111">
+        <v>5.6457</v>
+      </c>
+      <c r="D111">
+        <v>40</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>250</v>
+      </c>
+      <c r="G111">
+        <v>112</v>
+      </c>
+      <c r="H111">
+        <v>0.16</v>
+      </c>
+      <c r="I111">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112">
+        <v>-6</v>
+      </c>
+      <c r="B112">
+        <v>36</v>
+      </c>
+      <c r="C112">
+        <v>6.2205</v>
+      </c>
+      <c r="D112">
+        <v>40</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>250</v>
+      </c>
+      <c r="G112">
+        <v>112</v>
+      </c>
+      <c r="H112">
+        <v>0.16</v>
+      </c>
+      <c r="I112">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113">
+        <v>-5</v>
+      </c>
+      <c r="B113">
+        <v>36</v>
+      </c>
+      <c r="C113">
+        <v>6.6394</v>
+      </c>
+      <c r="D113">
+        <v>40</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>250</v>
+      </c>
+      <c r="G113">
+        <v>112</v>
+      </c>
+      <c r="H113">
+        <v>0.16</v>
+      </c>
+      <c r="I113">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="A114">
+        <v>-4</v>
+      </c>
+      <c r="B114">
+        <v>36</v>
+      </c>
+      <c r="C114">
+        <v>6.952000000000001</v>
+      </c>
+      <c r="D114">
+        <v>40</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <v>250</v>
+      </c>
+      <c r="G114">
+        <v>112</v>
+      </c>
+      <c r="H114">
+        <v>0.16</v>
+      </c>
+      <c r="I114">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115">
+        <v>-3</v>
+      </c>
+      <c r="B115">
+        <v>36</v>
+      </c>
+      <c r="C115">
+        <v>7.4017</v>
+      </c>
+      <c r="D115">
+        <v>40</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>250</v>
+      </c>
+      <c r="G115">
+        <v>112</v>
+      </c>
+      <c r="H115">
+        <v>0.16</v>
+      </c>
+      <c r="I115">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116">
+        <v>-2</v>
+      </c>
+      <c r="B116">
+        <v>36</v>
+      </c>
+      <c r="C116">
         <v>7.661</v>
       </c>
-      <c r="D94">
-        <v>40</v>
-      </c>
-      <c r="E94">
-        <v>0</v>
-      </c>
-      <c r="F94">
-        <v>250</v>
-      </c>
-      <c r="G94">
-        <v>112</v>
-      </c>
-      <c r="H94">
-        <v>0.16</v>
-      </c>
-      <c r="I94">
+      <c r="D116">
+        <v>40</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <v>250</v>
+      </c>
+      <c r="G116">
+        <v>112</v>
+      </c>
+      <c r="H116">
+        <v>0.16</v>
+      </c>
+      <c r="I116">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117">
+        <v>-1</v>
+      </c>
+      <c r="B117">
+        <v>36</v>
+      </c>
+      <c r="C117">
+        <v>7.5927</v>
+      </c>
+      <c r="D117">
+        <v>40</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117">
+        <v>250</v>
+      </c>
+      <c r="G117">
+        <v>112</v>
+      </c>
+      <c r="H117">
+        <v>0.16</v>
+      </c>
+      <c r="I117">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118">
+        <v>0</v>
+      </c>
+      <c r="B118">
+        <v>36</v>
+      </c>
+      <c r="C118">
+        <v>7.1499</v>
+      </c>
+      <c r="D118">
+        <v>40</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <v>250</v>
+      </c>
+      <c r="G118">
+        <v>112</v>
+      </c>
+      <c r="H118">
+        <v>0.16</v>
+      </c>
+      <c r="I118">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
+      <c r="A119">
+        <v>1</v>
+      </c>
+      <c r="B119">
+        <v>36</v>
+      </c>
+      <c r="C119">
+        <v>6.5137</v>
+      </c>
+      <c r="D119">
+        <v>40</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>250</v>
+      </c>
+      <c r="G119">
+        <v>112</v>
+      </c>
+      <c r="H119">
+        <v>0.16</v>
+      </c>
+      <c r="I119">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120">
+        <v>2</v>
+      </c>
+      <c r="B120">
+        <v>36</v>
+      </c>
+      <c r="C120">
+        <v>4.9084</v>
+      </c>
+      <c r="D120">
+        <v>40</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>250</v>
+      </c>
+      <c r="G120">
+        <v>112</v>
+      </c>
+      <c r="H120">
+        <v>0.16</v>
+      </c>
+      <c r="I120">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121">
+        <v>3</v>
+      </c>
+      <c r="B121">
+        <v>36</v>
+      </c>
+      <c r="C121">
+        <v>3.9518</v>
+      </c>
+      <c r="D121">
+        <v>40</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <v>250</v>
+      </c>
+      <c r="G121">
+        <v>112</v>
+      </c>
+      <c r="H121">
+        <v>0.16</v>
+      </c>
+      <c r="I121">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122">
+        <v>-8</v>
+      </c>
+      <c r="B122">
+        <v>40</v>
+      </c>
+      <c r="C122">
+        <v>5.0888</v>
+      </c>
+      <c r="D122">
+        <v>40</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <v>250</v>
+      </c>
+      <c r="G122">
+        <v>112</v>
+      </c>
+      <c r="H122">
+        <v>0.16</v>
+      </c>
+      <c r="I122">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123">
+        <v>-7</v>
+      </c>
+      <c r="B123">
+        <v>40</v>
+      </c>
+      <c r="C123">
+        <v>5.6105</v>
+      </c>
+      <c r="D123">
+        <v>40</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
+        <v>250</v>
+      </c>
+      <c r="G123">
+        <v>112</v>
+      </c>
+      <c r="H123">
+        <v>0.16</v>
+      </c>
+      <c r="I123">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124">
+        <v>-6</v>
+      </c>
+      <c r="B124">
+        <v>40</v>
+      </c>
+      <c r="C124">
+        <v>5.9827</v>
+      </c>
+      <c r="D124">
+        <v>40</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <v>250</v>
+      </c>
+      <c r="G124">
+        <v>112</v>
+      </c>
+      <c r="H124">
+        <v>0.16</v>
+      </c>
+      <c r="I124">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125">
+        <v>-5</v>
+      </c>
+      <c r="B125">
+        <v>40</v>
+      </c>
+      <c r="C125">
+        <v>6.5252</v>
+      </c>
+      <c r="D125">
+        <v>40</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <v>250</v>
+      </c>
+      <c r="G125">
+        <v>112</v>
+      </c>
+      <c r="H125">
+        <v>0.16</v>
+      </c>
+      <c r="I125">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126">
+        <v>-4</v>
+      </c>
+      <c r="B126">
+        <v>40</v>
+      </c>
+      <c r="C126">
+        <v>6.8922</v>
+      </c>
+      <c r="D126">
+        <v>40</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126">
+        <v>250</v>
+      </c>
+      <c r="G126">
+        <v>112</v>
+      </c>
+      <c r="H126">
+        <v>0.16</v>
+      </c>
+      <c r="I126">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127">
+        <v>-3</v>
+      </c>
+      <c r="B127">
+        <v>40</v>
+      </c>
+      <c r="C127">
+        <v>7.3465</v>
+      </c>
+      <c r="D127">
+        <v>40</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127">
+        <v>250</v>
+      </c>
+      <c r="G127">
+        <v>112</v>
+      </c>
+      <c r="H127">
+        <v>0.16</v>
+      </c>
+      <c r="I127">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
+      <c r="A128">
+        <v>-2</v>
+      </c>
+      <c r="B128">
+        <v>40</v>
+      </c>
+      <c r="C128">
+        <v>7.5763</v>
+      </c>
+      <c r="D128">
+        <v>40</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <v>250</v>
+      </c>
+      <c r="G128">
+        <v>112</v>
+      </c>
+      <c r="H128">
+        <v>0.16</v>
+      </c>
+      <c r="I128">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
+      <c r="A129">
+        <v>-1</v>
+      </c>
+      <c r="B129">
+        <v>40</v>
+      </c>
+      <c r="C129">
+        <v>7.4109</v>
+      </c>
+      <c r="D129">
+        <v>40</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <v>250</v>
+      </c>
+      <c r="G129">
+        <v>112</v>
+      </c>
+      <c r="H129">
+        <v>0.16</v>
+      </c>
+      <c r="I129">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
+      <c r="A130">
+        <v>0</v>
+      </c>
+      <c r="B130">
+        <v>40</v>
+      </c>
+      <c r="C130">
+        <v>7.3004</v>
+      </c>
+      <c r="D130">
+        <v>40</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <v>250</v>
+      </c>
+      <c r="G130">
+        <v>112</v>
+      </c>
+      <c r="H130">
+        <v>0.16</v>
+      </c>
+      <c r="I130">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="A131">
+        <v>1</v>
+      </c>
+      <c r="B131">
+        <v>40</v>
+      </c>
+      <c r="C131">
+        <v>6.7094</v>
+      </c>
+      <c r="D131">
+        <v>40</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <v>250</v>
+      </c>
+      <c r="G131">
+        <v>112</v>
+      </c>
+      <c r="H131">
+        <v>0.16</v>
+      </c>
+      <c r="I131">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132">
+        <v>2</v>
+      </c>
+      <c r="B132">
+        <v>40</v>
+      </c>
+      <c r="C132">
+        <v>5.7749</v>
+      </c>
+      <c r="D132">
+        <v>40</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132">
+        <v>250</v>
+      </c>
+      <c r="G132">
+        <v>112</v>
+      </c>
+      <c r="H132">
+        <v>0.16</v>
+      </c>
+      <c r="I132">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133">
+        <v>3</v>
+      </c>
+      <c r="B133">
+        <v>40</v>
+      </c>
+      <c r="C133">
+        <v>4.2639</v>
+      </c>
+      <c r="D133">
+        <v>40</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133">
+        <v>250</v>
+      </c>
+      <c r="G133">
+        <v>112</v>
+      </c>
+      <c r="H133">
+        <v>0.16</v>
+      </c>
+      <c r="I133">
         <v>0.158</v>
       </c>
     </row>

</xml_diff>